<commit_message>
Modified json file for Solis description
</commit_message>
<xml_diff>
--- a/mapping_tools/modbus_defs_dbnpoller.xlsx
+++ b/mapping_tools/modbus_defs_dbnpoller.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidbaldwin/Work/2020/DS008-2020 (B4E-BUILDING)/energy_poller/mapping_tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidbaldwin/Work/2020/DS008-2020 (B4E-BUILDING)/rpiB4e/energy_poller/mapping_tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C60922-7C37-4F4F-82F4-94713C9DFD86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CF474A-D450-B543-9583-357FE81C5DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26080" yWindow="2840" windowWidth="36520" windowHeight="17600" tabRatio="680" activeTab="1" xr2:uid="{36DBA9D7-9C64-4198-95D1-4A402342E7C5}"/>
+    <workbookView xWindow="22580" yWindow="8200" windowWidth="36520" windowHeight="17600" tabRatio="680" activeTab="11" xr2:uid="{36DBA9D7-9C64-4198-95D1-4A402342E7C5}"/>
   </bookViews>
   <sheets>
     <sheet name="!!__UserGuide" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="223">
   <si>
     <t>uint8</t>
   </si>
@@ -702,6 +702,9 @@
   </si>
   <si>
     <t>SOLIS_4G_3P_part1</t>
+  </si>
+  <si>
+    <t>DC I String 1</t>
   </si>
 </sst>
 </file>
@@ -3859,8 +3862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB619ED0-7523-2842-94EF-A4C7328309AF}">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4222,7 +4225,7 @@
         <v>197</v>
       </c>
       <c r="L13" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="M13">
         <v>3022</v>
@@ -5870,7 +5873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AE8953-78F7-4FA3-BF4C-2AE305CCB3DF}">
   <dimension ref="A1:E257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Janitza B23 Modbus
</commit_message>
<xml_diff>
--- a/mapping_tools/modbus_defs_dbnpoller.xlsx
+++ b/mapping_tools/modbus_defs_dbnpoller.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidbaldwin/Work/2020/DS008-2020 (B4E-BUILDING)/rpiB4e/energy_poller/mapping_tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidbaldwin/Work/2020/DS008-2020 (B4E-BUILDING)/github/energy_poller/mapping_tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB92F6C-7BD8-DA49-BB3E-12F0D06CF642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFA1437-36E0-1C40-B67E-95A616150DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3640" windowWidth="35840" windowHeight="17600" tabRatio="680" activeTab="11" xr2:uid="{36DBA9D7-9C64-4198-95D1-4A402342E7C5}"/>
+    <workbookView xWindow="2200" yWindow="2460" windowWidth="35840" windowHeight="17600" tabRatio="680" activeTab="12" xr2:uid="{36DBA9D7-9C64-4198-95D1-4A402342E7C5}"/>
   </bookViews>
   <sheets>
     <sheet name="!!__UserGuide" sheetId="8" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="OR_WE_514_part1_v1" sheetId="6" r:id="rId10"/>
     <sheet name="OR_WE_514_part2_v1" sheetId="12" r:id="rId11"/>
     <sheet name="SOLIS_4G_3P_part1_v1" sheetId="14" r:id="rId12"/>
+    <sheet name="JANITZA_B23_part1_v1" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="235">
   <si>
     <t>uint8</t>
   </si>
@@ -708,6 +709,39 @@
   </si>
   <si>
     <t>Yesterday energy</t>
+  </si>
+  <si>
+    <t>V12</t>
+  </si>
+  <si>
+    <t>V23</t>
+  </si>
+  <si>
+    <t>V31</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>I3</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Ptot</t>
+  </si>
+  <si>
+    <t>JANITZA_B23_part1</t>
   </si>
 </sst>
 </file>
@@ -3865,7 +3899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB619ED0-7523-2842-94EF-A4C7328309AF}">
   <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -5906,12 +5940,1650 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24831CC8-1DF2-5E4A-B3B0-AE1C40F7A6EA}">
+  <dimension ref="A1:M86"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="5" max="8" width="10.83203125" style="12"/>
+    <col min="12" max="12" width="18.83203125" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6">
+        <f t="shared" ref="D2:D51" si="0">IF(ISBLANK($B2),"",IF(ISNUMBER($D1),$D1,0)+IF(ISNUMBER($C1),$C1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" t="s">
+        <v>224</v>
+      </c>
+      <c r="M2">
+        <v>19006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="L3" t="s">
+        <v>225</v>
+      </c>
+      <c r="M3">
+        <v>19008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="6">
+        <f>IF(ISBLANK($B4),"",IFERROR(VLOOKUP(B4,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B4,LEN($B4)-FIND("$",$B4)))/2))</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="L4" t="s">
+        <v>226</v>
+      </c>
+      <c r="M4">
+        <v>19010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6">
+        <f>IF(ISBLANK($B5),"",IFERROR(VLOOKUP(B5,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B5,LEN($B5)-FIND("$",$B5)))/2))</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" t="s">
+        <v>227</v>
+      </c>
+      <c r="M5">
+        <v>19012</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="6">
+        <f>IF(ISBLANK($B6),"",IFERROR(VLOOKUP(B6,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B6,LEN($B6)-FIND("$",$B6)))/2))</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="L6" t="s">
+        <v>228</v>
+      </c>
+      <c r="M6">
+        <v>19014</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="6">
+        <f>IF(ISBLANK($B7),"",IFERROR(VLOOKUP(B7,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B7,LEN($B7)-FIND("$",$B7)))/2))</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="L7" t="s">
+        <v>229</v>
+      </c>
+      <c r="M7">
+        <v>19016</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="6">
+        <f>IF(ISBLANK($B8),"",IFERROR(VLOOKUP(B8,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B8,LEN($B8)-FIND("$",$B8)))/2))</f>
+        <v>2</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="L8" t="s">
+        <v>145</v>
+      </c>
+      <c r="M8">
+        <v>19018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="6">
+        <f>IF(ISBLANK($B9),"",IFERROR(VLOOKUP(B9,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B9,LEN($B9)-FIND("$",$B9)))/2))</f>
+        <v>2</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" t="s">
+        <v>230</v>
+      </c>
+      <c r="M9">
+        <v>19020</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6">
+        <f>IF(ISBLANK($B10),"",IFERROR(VLOOKUP(B10,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B10,LEN($B10)-FIND("$",$B10)))/2))</f>
+        <v>2</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" t="s">
+        <v>231</v>
+      </c>
+      <c r="M10">
+        <v>19022</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6">
+        <f>IF(ISBLANK($B11),"",IFERROR(VLOOKUP(B11,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B11,LEN($B11)-FIND("$",$B11)))/2))</f>
+        <v>2</v>
+      </c>
+      <c r="D11" s="6">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" t="s">
+        <v>232</v>
+      </c>
+      <c r="M11">
+        <v>19024</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>233</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="6">
+        <f>IF(ISBLANK($B12),"",IFERROR(VLOOKUP(B12,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B12,LEN($B12)-FIND("$",$B12)))/2))</f>
+        <v>2</v>
+      </c>
+      <c r="D12" s="6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L12" t="s">
+        <v>233</v>
+      </c>
+      <c r="M12">
+        <v>19026</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="6">
+        <f>IF(ISBLANK($B13),"",IFERROR(VLOOKUP(B13,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B13,LEN($B13)-FIND("$",$B13)))/2))</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="6">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14" s="6" t="str">
+        <f>IF(ISBLANK($B14),"",IFERROR(VLOOKUP(B14,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B14,LEN($B14)-FIND("$",$B14)))/2))</f>
+        <v/>
+      </c>
+      <c r="D14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+    </row>
+    <row r="15" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15" s="6" t="str">
+        <f>IF(ISBLANK($B15),"",IFERROR(VLOOKUP(B15,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B15,LEN($B15)-FIND("$",$B15)))/2))</f>
+        <v/>
+      </c>
+      <c r="D15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16" s="6" t="str">
+        <f>IF(ISBLANK($B16),"",IFERROR(VLOOKUP(B16,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B16,LEN($B16)-FIND("$",$B16)))/2))</f>
+        <v/>
+      </c>
+      <c r="D16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17" s="6" t="str">
+        <f>IF(ISBLANK($B17),"",IFERROR(VLOOKUP(B17,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B17,LEN($B17)-FIND("$",$B17)))/2))</f>
+        <v/>
+      </c>
+      <c r="D17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+    </row>
+    <row r="18" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18" s="6" t="str">
+        <f>IF(ISBLANK($B18),"",IFERROR(VLOOKUP(B18,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B18,LEN($B18)-FIND("$",$B18)))/2))</f>
+        <v/>
+      </c>
+      <c r="D18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+    </row>
+    <row r="19" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19" s="6" t="str">
+        <f>IF(ISBLANK($B19),"",IFERROR(VLOOKUP(B19,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B19,LEN($B19)-FIND("$",$B19)))/2))</f>
+        <v/>
+      </c>
+      <c r="D19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20" s="6" t="str">
+        <f>IF(ISBLANK($B20),"",IFERROR(VLOOKUP(B20,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B20,LEN($B20)-FIND("$",$B20)))/2))</f>
+        <v/>
+      </c>
+      <c r="D20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+    </row>
+    <row r="21" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21" s="6" t="str">
+        <f>IF(ISBLANK($B21),"",IFERROR(VLOOKUP(B21,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B21,LEN($B21)-FIND("$",$B21)))/2))</f>
+        <v/>
+      </c>
+      <c r="D21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+    </row>
+    <row r="22" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22" s="6" t="str">
+        <f>IF(ISBLANK($B22),"",IFERROR(VLOOKUP(B22,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B22,LEN($B22)-FIND("$",$B22)))/2))</f>
+        <v/>
+      </c>
+      <c r="D22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+    </row>
+    <row r="23" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23" s="6" t="str">
+        <f>IF(ISBLANK($B23),"",IFERROR(VLOOKUP(B23,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B23,LEN($B23)-FIND("$",$B23)))/2))</f>
+        <v/>
+      </c>
+      <c r="D23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+    </row>
+    <row r="24" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24" s="6" t="str">
+        <f>IF(ISBLANK($B24),"",IFERROR(VLOOKUP(B24,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B24,LEN($B24)-FIND("$",$B24)))/2))</f>
+        <v/>
+      </c>
+      <c r="D24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+    </row>
+    <row r="25" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25" s="6" t="str">
+        <f>IF(ISBLANK($B25),"",IFERROR(VLOOKUP(B25,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B25,LEN($B25)-FIND("$",$B25)))/2))</f>
+        <v/>
+      </c>
+      <c r="D25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+    </row>
+    <row r="26" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26" s="6" t="str">
+        <f>IF(ISBLANK($B26),"",IFERROR(VLOOKUP(B26,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B26,LEN($B26)-FIND("$",$B26)))/2))</f>
+        <v/>
+      </c>
+      <c r="D26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+    </row>
+    <row r="27" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27" s="6" t="str">
+        <f>IF(ISBLANK($B27),"",IFERROR(VLOOKUP(B27,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B27,LEN($B27)-FIND("$",$B27)))/2))</f>
+        <v/>
+      </c>
+      <c r="D27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+    </row>
+    <row r="28" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28" s="6" t="str">
+        <f>IF(ISBLANK($B28),"",IFERROR(VLOOKUP(B28,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B28,LEN($B28)-FIND("$",$B28)))/2))</f>
+        <v/>
+      </c>
+      <c r="D28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+    </row>
+    <row r="29" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29" s="6" t="str">
+        <f>IF(ISBLANK($B29),"",IFERROR(VLOOKUP(B29,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B29,LEN($B29)-FIND("$",$B29)))/2))</f>
+        <v/>
+      </c>
+      <c r="D29" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+    </row>
+    <row r="30" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30" s="6" t="str">
+        <f>IF(ISBLANK($B30),"",IFERROR(VLOOKUP(B30,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B30,LEN($B30)-FIND("$",$B30)))/2))</f>
+        <v/>
+      </c>
+      <c r="D30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+    </row>
+    <row r="31" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31" s="6" t="str">
+        <f>IF(ISBLANK($B31),"",IFERROR(VLOOKUP(B31,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B31,LEN($B31)-FIND("$",$B31)))/2))</f>
+        <v/>
+      </c>
+      <c r="D31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+    </row>
+    <row r="32" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32" s="6" t="str">
+        <f>IF(ISBLANK($B32),"",IFERROR(VLOOKUP(B32,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B32,LEN($B32)-FIND("$",$B32)))/2))</f>
+        <v/>
+      </c>
+      <c r="D32" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+    </row>
+    <row r="33" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33" s="6" t="str">
+        <f>IF(ISBLANK($B33),"",IFERROR(VLOOKUP(B33,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B33,LEN($B33)-FIND("$",$B33)))/2))</f>
+        <v/>
+      </c>
+      <c r="D33" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+    </row>
+    <row r="34" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34" s="6" t="str">
+        <f>IF(ISBLANK($B34),"",IFERROR(VLOOKUP(B34,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B34,LEN($B34)-FIND("$",$B34)))/2))</f>
+        <v/>
+      </c>
+      <c r="D34" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+    </row>
+    <row r="35" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35" s="6" t="str">
+        <f>IF(ISBLANK($B35),"",IFERROR(VLOOKUP(B35,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B35,LEN($B35)-FIND("$",$B35)))/2))</f>
+        <v/>
+      </c>
+      <c r="D35" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+    </row>
+    <row r="36" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36" s="6" t="str">
+        <f>IF(ISBLANK($B36),"",IFERROR(VLOOKUP(B36,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B36,LEN($B36)-FIND("$",$B36)))/2))</f>
+        <v/>
+      </c>
+      <c r="D36" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+    </row>
+    <row r="37" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37" s="6" t="str">
+        <f>IF(ISBLANK($B37),"",IFERROR(VLOOKUP(B37,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B37,LEN($B37)-FIND("$",$B37)))/2))</f>
+        <v/>
+      </c>
+      <c r="D37" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+    </row>
+    <row r="38" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38" s="6" t="str">
+        <f>IF(ISBLANK($B38),"",IFERROR(VLOOKUP(B38,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B38,LEN($B38)-FIND("$",$B38)))/2))</f>
+        <v/>
+      </c>
+      <c r="D38" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+    </row>
+    <row r="39" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39"/>
+      <c r="B39"/>
+      <c r="C39" s="6" t="str">
+        <f>IF(ISBLANK($B39),"",IFERROR(VLOOKUP(B39,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B39,LEN($B39)-FIND("$",$B39)))/2))</f>
+        <v/>
+      </c>
+      <c r="D39" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+    </row>
+    <row r="40" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40"/>
+      <c r="B40"/>
+      <c r="C40" s="6" t="str">
+        <f>IF(ISBLANK($B40),"",IFERROR(VLOOKUP(B40,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B40,LEN($B40)-FIND("$",$B40)))/2))</f>
+        <v/>
+      </c>
+      <c r="D40" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+    </row>
+    <row r="41" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41" s="6" t="str">
+        <f>IF(ISBLANK($B41),"",IFERROR(VLOOKUP(B41,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B41,LEN($B41)-FIND("$",$B41)))/2))</f>
+        <v/>
+      </c>
+      <c r="D41" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+    </row>
+    <row r="42" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42"/>
+      <c r="B42"/>
+      <c r="C42" s="6" t="str">
+        <f>IF(ISBLANK($B42),"",IFERROR(VLOOKUP(B42,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B42,LEN($B42)-FIND("$",$B42)))/2))</f>
+        <v/>
+      </c>
+      <c r="D42" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+    </row>
+    <row r="43" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43" s="6" t="str">
+        <f>IF(ISBLANK($B43),"",IFERROR(VLOOKUP(B43,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B43,LEN($B43)-FIND("$",$B43)))/2))</f>
+        <v/>
+      </c>
+      <c r="D43" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+    </row>
+    <row r="44" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44" s="6" t="str">
+        <f>IF(ISBLANK($B44),"",IFERROR(VLOOKUP(B44,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B44,LEN($B44)-FIND("$",$B44)))/2))</f>
+        <v/>
+      </c>
+      <c r="D44" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+    </row>
+    <row r="45" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45"/>
+      <c r="B45"/>
+      <c r="C45" s="6" t="str">
+        <f>IF(ISBLANK($B45),"",IFERROR(VLOOKUP(B45,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B45,LEN($B45)-FIND("$",$B45)))/2))</f>
+        <v/>
+      </c>
+      <c r="D45" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+    </row>
+    <row r="46" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46"/>
+      <c r="B46"/>
+      <c r="C46" s="6" t="str">
+        <f>IF(ISBLANK($B46),"",IFERROR(VLOOKUP(B46,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B46,LEN($B46)-FIND("$",$B46)))/2))</f>
+        <v/>
+      </c>
+      <c r="D46" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+    </row>
+    <row r="47" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47"/>
+      <c r="B47"/>
+      <c r="C47" s="6" t="str">
+        <f>IF(ISBLANK($B47),"",IFERROR(VLOOKUP(B47,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B47,LEN($B47)-FIND("$",$B47)))/2))</f>
+        <v/>
+      </c>
+      <c r="D47" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+    </row>
+    <row r="48" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48" s="6" t="str">
+        <f>IF(ISBLANK($B48),"",IFERROR(VLOOKUP(B48,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B48,LEN($B48)-FIND("$",$B48)))/2))</f>
+        <v/>
+      </c>
+      <c r="D48" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+    </row>
+    <row r="49" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49"/>
+      <c r="B49"/>
+      <c r="C49" s="6" t="str">
+        <f>IF(ISBLANK($B49),"",IFERROR(VLOOKUP(B49,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B49,LEN($B49)-FIND("$",$B49)))/2))</f>
+        <v/>
+      </c>
+      <c r="D49" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
+    </row>
+    <row r="50" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50"/>
+      <c r="B50"/>
+      <c r="C50" s="6" t="str">
+        <f>IF(ISBLANK($B50),"",IFERROR(VLOOKUP(B50,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B50,LEN($B50)-FIND("$",$B50)))/2))</f>
+        <v/>
+      </c>
+      <c r="D50" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+    </row>
+    <row r="51" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51"/>
+      <c r="B51"/>
+      <c r="C51" s="6" t="str">
+        <f>IF(ISBLANK($B51),"",IFERROR(VLOOKUP(B51,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B51,LEN($B51)-FIND("$",$B51)))/2))</f>
+        <v/>
+      </c>
+      <c r="D51" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+    </row>
+    <row r="52" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52"/>
+      <c r="B52"/>
+      <c r="C52" s="6" t="str">
+        <f>IF(ISBLANK($B52),"",IFERROR(VLOOKUP(B52,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B52,LEN($B52)-FIND("$",$B52)))/2))</f>
+        <v/>
+      </c>
+      <c r="D52" s="6" t="str">
+        <f t="shared" ref="D52:D86" si="1">IF(ISBLANK($B52),"",IF(ISNUMBER($D51),$D51,0)+IF(ISNUMBER($C51),$C51,0))</f>
+        <v/>
+      </c>
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+    </row>
+    <row r="53" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53"/>
+      <c r="B53"/>
+      <c r="C53" s="6" t="str">
+        <f>IF(ISBLANK($B53),"",IFERROR(VLOOKUP(B53,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B53,LEN($B53)-FIND("$",$B53)))/2))</f>
+        <v/>
+      </c>
+      <c r="D53" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+    </row>
+    <row r="54" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54"/>
+      <c r="B54"/>
+      <c r="C54" s="6" t="str">
+        <f>IF(ISBLANK($B54),"",IFERROR(VLOOKUP(B54,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B54,LEN($B54)-FIND("$",$B54)))/2))</f>
+        <v/>
+      </c>
+      <c r="D54" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+    </row>
+    <row r="55" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55"/>
+      <c r="B55"/>
+      <c r="C55" s="6" t="str">
+        <f>IF(ISBLANK($B55),"",IFERROR(VLOOKUP(B55,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B55,LEN($B55)-FIND("$",$B55)))/2))</f>
+        <v/>
+      </c>
+      <c r="D55" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+    </row>
+    <row r="56" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56"/>
+      <c r="B56"/>
+      <c r="C56" s="6" t="str">
+        <f>IF(ISBLANK($B56),"",IFERROR(VLOOKUP(B56,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B56,LEN($B56)-FIND("$",$B56)))/2))</f>
+        <v/>
+      </c>
+      <c r="D56" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+    </row>
+    <row r="57" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57"/>
+      <c r="B57"/>
+      <c r="C57" s="6" t="str">
+        <f>IF(ISBLANK($B57),"",IFERROR(VLOOKUP(B57,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B57,LEN($B57)-FIND("$",$B57)))/2))</f>
+        <v/>
+      </c>
+      <c r="D57" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+    </row>
+    <row r="58" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58"/>
+      <c r="B58"/>
+      <c r="C58" s="6" t="str">
+        <f>IF(ISBLANK($B58),"",IFERROR(VLOOKUP(B58,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B58,LEN($B58)-FIND("$",$B58)))/2))</f>
+        <v/>
+      </c>
+      <c r="D58" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
+    </row>
+    <row r="59" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59"/>
+      <c r="B59"/>
+      <c r="C59" s="6" t="str">
+        <f>IF(ISBLANK($B59),"",IFERROR(VLOOKUP(B59,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B59,LEN($B59)-FIND("$",$B59)))/2))</f>
+        <v/>
+      </c>
+      <c r="D59" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I59"/>
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="M59"/>
+    </row>
+    <row r="60" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60"/>
+      <c r="B60"/>
+      <c r="C60" s="6" t="str">
+        <f>IF(ISBLANK($B60),"",IFERROR(VLOOKUP(B60,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B60,LEN($B60)-FIND("$",$B60)))/2))</f>
+        <v/>
+      </c>
+      <c r="D60" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I60"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+    </row>
+    <row r="61" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61"/>
+      <c r="B61"/>
+      <c r="C61" s="6" t="str">
+        <f>IF(ISBLANK($B61),"",IFERROR(VLOOKUP(B61,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B61,LEN($B61)-FIND("$",$B61)))/2))</f>
+        <v/>
+      </c>
+      <c r="D61" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I61"/>
+      <c r="J61"/>
+      <c r="K61"/>
+      <c r="L61"/>
+      <c r="M61"/>
+    </row>
+    <row r="62" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62"/>
+      <c r="B62"/>
+      <c r="C62" s="6" t="str">
+        <f>IF(ISBLANK($B62),"",IFERROR(VLOOKUP(B62,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B62,LEN($B62)-FIND("$",$B62)))/2))</f>
+        <v/>
+      </c>
+      <c r="D62" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I62"/>
+      <c r="J62"/>
+      <c r="K62"/>
+      <c r="L62"/>
+      <c r="M62"/>
+    </row>
+    <row r="63" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63"/>
+      <c r="B63"/>
+      <c r="C63" s="6" t="str">
+        <f>IF(ISBLANK($B63),"",IFERROR(VLOOKUP(B63,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B63,LEN($B63)-FIND("$",$B63)))/2))</f>
+        <v/>
+      </c>
+      <c r="D63" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I63"/>
+      <c r="J63"/>
+      <c r="K63"/>
+      <c r="L63"/>
+      <c r="M63"/>
+    </row>
+    <row r="64" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64"/>
+      <c r="B64"/>
+      <c r="C64" s="6" t="str">
+        <f>IF(ISBLANK($B64),"",IFERROR(VLOOKUP(B64,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B64,LEN($B64)-FIND("$",$B64)))/2))</f>
+        <v/>
+      </c>
+      <c r="D64" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I64"/>
+      <c r="J64"/>
+      <c r="K64"/>
+      <c r="L64"/>
+      <c r="M64"/>
+    </row>
+    <row r="65" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65"/>
+      <c r="B65"/>
+      <c r="C65" s="6" t="str">
+        <f>IF(ISBLANK($B65),"",IFERROR(VLOOKUP(B65,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B65,LEN($B65)-FIND("$",$B65)))/2))</f>
+        <v/>
+      </c>
+      <c r="D65" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I65"/>
+      <c r="J65"/>
+      <c r="K65"/>
+      <c r="L65"/>
+      <c r="M65"/>
+    </row>
+    <row r="66" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66"/>
+      <c r="B66"/>
+      <c r="C66" s="6" t="str">
+        <f>IF(ISBLANK($B66),"",IFERROR(VLOOKUP(B66,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B66,LEN($B66)-FIND("$",$B66)))/2))</f>
+        <v/>
+      </c>
+      <c r="D66" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I66"/>
+      <c r="J66"/>
+      <c r="K66"/>
+      <c r="L66"/>
+      <c r="M66"/>
+    </row>
+    <row r="67" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67"/>
+      <c r="B67"/>
+      <c r="C67" s="6" t="str">
+        <f>IF(ISBLANK($B67),"",IFERROR(VLOOKUP(B67,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B67,LEN($B67)-FIND("$",$B67)))/2))</f>
+        <v/>
+      </c>
+      <c r="D67" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I67"/>
+      <c r="J67"/>
+      <c r="K67"/>
+      <c r="L67"/>
+      <c r="M67"/>
+    </row>
+    <row r="68" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68"/>
+      <c r="B68"/>
+      <c r="C68" s="6" t="str">
+        <f>IF(ISBLANK($B68),"",IFERROR(VLOOKUP(B68,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B68,LEN($B68)-FIND("$",$B68)))/2))</f>
+        <v/>
+      </c>
+      <c r="D68" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I68"/>
+      <c r="J68"/>
+      <c r="K68"/>
+      <c r="L68"/>
+      <c r="M68"/>
+    </row>
+    <row r="69" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69"/>
+      <c r="B69"/>
+      <c r="C69" s="6" t="str">
+        <f>IF(ISBLANK($B69),"",IFERROR(VLOOKUP(B69,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B69,LEN($B69)-FIND("$",$B69)))/2))</f>
+        <v/>
+      </c>
+      <c r="D69" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I69"/>
+      <c r="J69"/>
+      <c r="K69"/>
+      <c r="L69"/>
+      <c r="M69"/>
+    </row>
+    <row r="70" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70"/>
+      <c r="B70"/>
+      <c r="C70" s="6" t="str">
+        <f>IF(ISBLANK($B70),"",IFERROR(VLOOKUP(B70,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B70,LEN($B70)-FIND("$",$B70)))/2))</f>
+        <v/>
+      </c>
+      <c r="D70" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I70"/>
+      <c r="J70"/>
+      <c r="K70"/>
+      <c r="L70"/>
+      <c r="M70"/>
+    </row>
+    <row r="71" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71"/>
+      <c r="B71"/>
+      <c r="C71" s="6" t="str">
+        <f>IF(ISBLANK($B71),"",IFERROR(VLOOKUP(B71,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B71,LEN($B71)-FIND("$",$B71)))/2))</f>
+        <v/>
+      </c>
+      <c r="D71" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I71"/>
+      <c r="J71"/>
+      <c r="K71"/>
+      <c r="L71"/>
+      <c r="M71"/>
+    </row>
+    <row r="72" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72"/>
+      <c r="B72"/>
+      <c r="C72" s="6" t="str">
+        <f>IF(ISBLANK($B72),"",IFERROR(VLOOKUP(B72,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B72,LEN($B72)-FIND("$",$B72)))/2))</f>
+        <v/>
+      </c>
+      <c r="D72" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I72"/>
+      <c r="J72"/>
+      <c r="K72"/>
+      <c r="L72"/>
+      <c r="M72"/>
+    </row>
+    <row r="73" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73"/>
+      <c r="B73"/>
+      <c r="C73" s="6" t="str">
+        <f>IF(ISBLANK($B73),"",IFERROR(VLOOKUP(B73,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B73,LEN($B73)-FIND("$",$B73)))/2))</f>
+        <v/>
+      </c>
+      <c r="D73" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I73"/>
+      <c r="J73"/>
+      <c r="K73"/>
+      <c r="L73"/>
+      <c r="M73"/>
+    </row>
+    <row r="74" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74"/>
+      <c r="B74"/>
+      <c r="C74" s="6" t="str">
+        <f>IF(ISBLANK($B74),"",IFERROR(VLOOKUP(B74,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B74,LEN($B74)-FIND("$",$B74)))/2))</f>
+        <v/>
+      </c>
+      <c r="D74" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I74"/>
+      <c r="J74"/>
+      <c r="K74"/>
+      <c r="L74"/>
+      <c r="M74"/>
+    </row>
+    <row r="75" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75"/>
+      <c r="B75"/>
+      <c r="C75" s="6" t="str">
+        <f>IF(ISBLANK($B75),"",IFERROR(VLOOKUP(B75,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B75,LEN($B75)-FIND("$",$B75)))/2))</f>
+        <v/>
+      </c>
+      <c r="D75" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I75"/>
+      <c r="J75"/>
+      <c r="K75"/>
+      <c r="L75"/>
+      <c r="M75"/>
+    </row>
+    <row r="76" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76"/>
+      <c r="B76"/>
+      <c r="C76" s="6" t="str">
+        <f>IF(ISBLANK($B76),"",IFERROR(VLOOKUP(B76,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B76,LEN($B76)-FIND("$",$B76)))/2))</f>
+        <v/>
+      </c>
+      <c r="D76" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I76"/>
+      <c r="J76"/>
+      <c r="K76"/>
+      <c r="L76"/>
+      <c r="M76"/>
+    </row>
+    <row r="77" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77"/>
+      <c r="B77"/>
+      <c r="C77" s="6" t="str">
+        <f>IF(ISBLANK($B77),"",IFERROR(VLOOKUP(B77,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B77,LEN($B77)-FIND("$",$B77)))/2))</f>
+        <v/>
+      </c>
+      <c r="D77" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I77"/>
+      <c r="J77"/>
+      <c r="K77"/>
+      <c r="L77"/>
+      <c r="M77"/>
+    </row>
+    <row r="78" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78"/>
+      <c r="B78"/>
+      <c r="C78" s="6" t="str">
+        <f>IF(ISBLANK($B78),"",IFERROR(VLOOKUP(B78,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B78,LEN($B78)-FIND("$",$B78)))/2))</f>
+        <v/>
+      </c>
+      <c r="D78" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I78"/>
+      <c r="J78"/>
+      <c r="K78"/>
+      <c r="L78"/>
+      <c r="M78"/>
+    </row>
+    <row r="79" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79"/>
+      <c r="B79"/>
+      <c r="C79" s="6" t="str">
+        <f>IF(ISBLANK($B79),"",IFERROR(VLOOKUP(B79,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B79,LEN($B79)-FIND("$",$B79)))/2))</f>
+        <v/>
+      </c>
+      <c r="D79" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I79"/>
+      <c r="J79"/>
+      <c r="K79"/>
+      <c r="L79"/>
+      <c r="M79"/>
+    </row>
+    <row r="80" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80"/>
+      <c r="B80"/>
+      <c r="C80" s="6" t="str">
+        <f>IF(ISBLANK($B80),"",IFERROR(VLOOKUP(B80,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B80,LEN($B80)-FIND("$",$B80)))/2))</f>
+        <v/>
+      </c>
+      <c r="D80" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I80"/>
+      <c r="J80"/>
+      <c r="K80"/>
+      <c r="L80"/>
+      <c r="M80"/>
+    </row>
+    <row r="81" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81"/>
+      <c r="B81"/>
+      <c r="C81" s="6" t="str">
+        <f>IF(ISBLANK($B81),"",IFERROR(VLOOKUP(B81,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B81,LEN($B81)-FIND("$",$B81)))/2))</f>
+        <v/>
+      </c>
+      <c r="D81" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I81"/>
+      <c r="J81"/>
+      <c r="K81"/>
+      <c r="L81"/>
+      <c r="M81"/>
+    </row>
+    <row r="82" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82"/>
+      <c r="B82"/>
+      <c r="C82" s="6" t="str">
+        <f>IF(ISBLANK($B82),"",IFERROR(VLOOKUP(B82,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B82,LEN($B82)-FIND("$",$B82)))/2))</f>
+        <v/>
+      </c>
+      <c r="D82" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I82"/>
+      <c r="J82"/>
+      <c r="K82"/>
+      <c r="L82"/>
+      <c r="M82"/>
+    </row>
+    <row r="83" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83"/>
+      <c r="B83"/>
+      <c r="C83" s="6" t="str">
+        <f>IF(ISBLANK($B83),"",IFERROR(VLOOKUP(B83,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B83,LEN($B83)-FIND("$",$B83)))/2))</f>
+        <v/>
+      </c>
+      <c r="D83" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I83"/>
+      <c r="J83"/>
+      <c r="K83"/>
+      <c r="L83"/>
+      <c r="M83"/>
+    </row>
+    <row r="84" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84"/>
+      <c r="B84"/>
+      <c r="C84" s="6" t="str">
+        <f>IF(ISBLANK($B84),"",IFERROR(VLOOKUP(B84,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B84,LEN($B84)-FIND("$",$B84)))/2))</f>
+        <v/>
+      </c>
+      <c r="D84" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I84"/>
+      <c r="J84"/>
+      <c r="K84"/>
+      <c r="L84"/>
+      <c r="M84"/>
+    </row>
+    <row r="85" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85"/>
+      <c r="B85"/>
+      <c r="C85" s="6" t="str">
+        <f>IF(ISBLANK($B85),"",IFERROR(VLOOKUP(B85,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B85,LEN($B85)-FIND("$",$B85)))/2))</f>
+        <v/>
+      </c>
+      <c r="D85" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I85"/>
+      <c r="J85"/>
+      <c r="K85"/>
+      <c r="L85"/>
+      <c r="M85"/>
+    </row>
+    <row r="86" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86"/>
+      <c r="B86"/>
+      <c r="C86" s="6" t="str">
+        <f>IF(ISBLANK($B86),"",IFERROR(VLOOKUP(B86,__Types!$A$3:$C$16,3,FALSE),VALUE(RIGHT($B86,LEN($B86)-FIND("$",$B86)))/2))</f>
+        <v/>
+      </c>
+      <c r="D86" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I86"/>
+      <c r="J86"/>
+      <c r="K86"/>
+      <c r="L86"/>
+      <c r="M86"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9DF03BEF-0672-BE40-B717-450E7F8B0594}">
+          <x14:formula1>
+            <xm:f>__Types!$A$3:$A$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B86</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4733FEF4-474A-7F40-98C6-B81203CB1921}">
+          <x14:formula1>
+            <xm:f>__AccessModes!$A$3:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E86</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AE8953-78F7-4FA3-BF4C-2AE305CCB3DF}">
   <dimension ref="A1:E257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6052,9 +7724,18 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D9" s="13" t="str">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13">
         <f t="shared" ref="D9:D72" ca="1" si="1">IF(ISBLANK($B9),"",IFERROR(MAX(INDIRECT(""&amp;$B9&amp;"_v"&amp;$C9&amp;"!$D:$D")),"bad ref"))</f>
-        <v/>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -9910,7 +11591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B7A809-83E4-4BE9-9792-B92CC13CBB5D}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>

</xml_diff>